<commit_message>
tfs6377 - ecl break feed for qs and sups
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C37142
</commit_message>
<xml_diff>
--- a/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
+++ b/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a_wip\ecl\doc\tfs_changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Requirements\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="133">
   <si>
     <t>CSR</t>
   </si>
@@ -346,11 +346,6 @@
 Research Required</t>
   </si>
   <si>
-    <t>OMR
-(IAE,IAT)
-Research Required</t>
-  </si>
-  <si>
     <t>tfs2470 - eCL Mass log load</t>
   </si>
   <si>
@@ -433,6 +428,37 @@
   </si>
   <si>
     <t>TFS5149 - eCL Requirement Document Cleanup</t>
+  </si>
+  <si>
+    <t>OMR
+(IAE,IAT,BRL,BRN)
+Research Required</t>
+  </si>
+  <si>
+    <t>Log Generation</t>
+  </si>
+  <si>
+    <t>Internal CCO Reporting
+(NPN)
+Opportunity</t>
+  </si>
+  <si>
+    <t>Performance Scorecard
+(MSRS)
+Reinforcement</t>
+  </si>
+  <si>
+    <t>Performance Scorecard
+(MSR)
+Reinforcement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal CCO Reporting
+(BRN, BRL)
+Opportunity </t>
+  </si>
+  <si>
+    <t>tfs6377 - ecl break feed for qs &amp; sups and other</t>
   </si>
 </sst>
 </file>
@@ -541,7 +567,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -601,11 +627,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -737,6 +772,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -770,11 +814,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1100,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E16"/>
+  <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1287,7 +1343,7 @@
         <v>42471</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14">
         <v>1.1200000000000001</v>
@@ -1301,7 +1357,7 @@
         <v>42563</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D15">
         <v>1.1299999999999999</v>
@@ -1315,12 +1371,26 @@
         <v>42375</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D16">
         <v>1.1399999999999999</v>
       </c>
       <c r="E16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="23">
+        <v>42845</v>
+      </c>
+      <c r="C17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E17" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1331,13 +1401,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1382,19 +1452,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1432,10 +1502,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="38" t="s">
@@ -1467,8 +1537,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="66"/>
-      <c r="B9" s="67"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="52" t="s">
         <v>6</v>
       </c>
@@ -1498,8 +1568,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="70"/>
       <c r="C10" s="6" t="s">
         <v>6</v>
       </c>
@@ -1529,8 +1599,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="66"/>
-      <c r="B11" s="67"/>
+      <c r="A11" s="69"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="40" t="s">
         <v>6</v>
       </c>
@@ -1560,8 +1630,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="66"/>
-      <c r="B12" s="62"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="25" t="s">
         <v>10</v>
       </c>
@@ -1591,8 +1661,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="66"/>
-      <c r="B13" s="61" t="s">
+      <c r="A13" s="69"/>
+      <c r="B13" s="64" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="34" t="s">
@@ -1624,8 +1694,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="66"/>
-      <c r="B14" s="67"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="52" t="s">
         <v>6</v>
       </c>
@@ -1668,20 +1738,20 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="63" t="s">
+      <c r="A16" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="69" t="s">
+      <c r="C16" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="70" t="s">
-        <v>101</v>
+      <c r="E16" s="39" t="s">
+        <v>130</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>58</v>
@@ -1699,15 +1769,17 @@
         <v>83</v>
       </c>
       <c r="K16" s="39" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="71"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="61" t="s">
+        <v>101</v>
+      </c>
       <c r="F17" s="32" t="s">
         <v>56</v>
       </c>
@@ -1728,12 +1800,12 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="64"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="69"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="46" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="F18" s="34" t="s">
         <v>57</v>
@@ -1754,11 +1826,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="64"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="69"/>
+    <row r="19" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="67"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="72"/>
       <c r="E19" s="57" t="s">
         <v>102</v>
       </c>
@@ -1795,10 +1867,10 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="64" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" s="63" t="s">
+      <c r="A21" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="66" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1826,12 +1898,12 @@
         <v>51</v>
       </c>
       <c r="K21" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
-      <c r="B22" s="63"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="34" t="s">
         <v>54</v>
       </c>
@@ -1861,13 +1933,13 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A23" s="64"/>
-      <c r="B23" s="63"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="52" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E23" s="53" t="s">
         <v>27</v>
@@ -1905,10 +1977,10 @@
       <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" s="61" t="s">
+      <c r="A25" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="64" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="34" t="s">
@@ -1940,8 +2012,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="60"/>
-      <c r="B26" s="62"/>
+      <c r="A26" s="63"/>
+      <c r="B26" s="65"/>
       <c r="C26" s="54" t="s">
         <v>54</v>
       </c>
@@ -1972,7 +2044,7 @@
     </row>
     <row r="28" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="44" t="s">
         <v>18</v>
@@ -1984,7 +2056,7 @@
         <v>28</v>
       </c>
       <c r="E28" s="35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F28" s="34" t="s">
         <v>57</v>
@@ -2007,7 +2079,7 @@
     </row>
     <row r="30" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="44" t="s">
         <v>18</v>
@@ -2019,7 +2091,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F30" s="38" t="s">
         <v>58</v>
@@ -2037,12 +2109,12 @@
         <v>51</v>
       </c>
       <c r="K30" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B32" s="47" t="s">
         <v>18</v>
@@ -2054,7 +2126,7 @@
         <v>6</v>
       </c>
       <c r="E32" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F32" s="38" t="s">
         <v>58</v>
@@ -2072,11 +2144,46 @@
         <v>51</v>
       </c>
       <c r="K32" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="J34" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="35" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B21:B23"/>
@@ -2089,7 +2196,6 @@
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="C16:C19"/>
     <mergeCell ref="D16:D19"/>
-    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2098,7 +2204,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
@@ -2148,19 +2254,19 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2198,10 +2304,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="52" t="s">
@@ -2233,8 +2339,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="64"/>
-      <c r="B9" s="67"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="40" t="s">
         <v>6</v>
       </c>
@@ -2264,8 +2370,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="64"/>
-      <c r="B10" s="62"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="25" t="s">
         <v>10</v>
       </c>
@@ -2295,8 +2401,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="64"/>
-      <c r="B11" s="63" t="s">
+      <c r="A11" s="67"/>
+      <c r="B11" s="66" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -2328,8 +2434,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="64"/>
-      <c r="B12" s="63"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="52" t="s">
         <v>6</v>
       </c>
@@ -2372,10 +2478,10 @@
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="61" t="s">
+      <c r="A14" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="64" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="34" t="s">
@@ -2408,8 +2514,8 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="60"/>
-      <c r="B15" s="62"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="54" t="s">
         <v>54</v>
       </c>
@@ -2441,7 +2547,7 @@
     </row>
     <row r="17" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" s="47" t="s">
         <v>18</v>
@@ -2453,7 +2559,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F17" s="38" t="s">
         <v>58</v>
@@ -2471,11 +2577,77 @@
         <v>51</v>
       </c>
       <c r="K17" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="36" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" s="39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="74"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B11:B12"/>
@@ -2490,13 +2662,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8:B9"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2539,19 +2711,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2589,10 +2761,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="80" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -2624,8 +2796,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="72"/>
-      <c r="B9" s="74"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="25" t="s">
         <v>10</v>
       </c>
@@ -2655,7 +2827,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="72"/>
+      <c r="A10" s="79"/>
       <c r="B10" s="15" t="s">
         <v>18</v>
       </c>
@@ -2699,6 +2871,41 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
+    </row>
+    <row r="12" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="35" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2759,19 +2966,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2809,10 +3016,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="80" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -2844,8 +3051,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="72"/>
-      <c r="B9" s="74"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="25" t="s">
         <v>10</v>
       </c>
@@ -2875,7 +3082,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="72"/>
+      <c r="A10" s="79"/>
       <c r="B10" s="15" t="s">
         <v>18</v>
       </c>
@@ -3032,19 +3239,19 @@
       <c r="K5" s="36"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
@@ -3082,10 +3289,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="80" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -3117,8 +3324,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="72"/>
-      <c r="B9" s="76"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="52" t="s">
         <v>54</v>
       </c>
@@ -3148,8 +3355,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="72"/>
-      <c r="B10" s="74"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="25" t="s">
         <v>10</v>
       </c>
@@ -3179,8 +3386,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="72"/>
-      <c r="B11" s="75" t="s">
+      <c r="A11" s="79"/>
+      <c r="B11" s="82" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -3212,8 +3419,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="72"/>
-      <c r="B12" s="75"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="82"/>
       <c r="C12" s="52" t="s">
         <v>54</v>
       </c>
@@ -3322,19 +3529,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
@@ -3372,17 +3579,17 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="63" t="s">
+      <c r="A8" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="66" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>25</v>
@@ -3403,17 +3610,17 @@
         <v>51</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="64"/>
-      <c r="B9" s="63"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="40" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="40" t="s">
         <v>25</v>
@@ -3438,13 +3645,13 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="64"/>
-      <c r="B10" s="63"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="34" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>25</v>
@@ -3469,13 +3676,13 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="64"/>
-      <c r="B11" s="63"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="52" t="s">
         <v>54</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" s="53" t="s">
         <v>25</v>
@@ -3513,17 +3720,17 @@
       <c r="K12" s="43"/>
     </row>
     <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="63" t="s">
+      <c r="A13" s="67" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="66" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>54</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E13" s="39" t="s">
         <v>25</v>
@@ -3544,17 +3751,17 @@
         <v>51</v>
       </c>
       <c r="K13" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="64"/>
-      <c r="B14" s="63"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="40" t="s">
         <v>54</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E14" s="40" t="s">
         <v>25</v>
@@ -3579,13 +3786,13 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="64"/>
-      <c r="B15" s="63"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="34" t="s">
         <v>54</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>25</v>
@@ -3610,13 +3817,13 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="64"/>
-      <c r="B16" s="63"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="52" t="s">
         <v>54</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E16" s="53" t="s">
         <v>25</v>
@@ -3654,17 +3861,17 @@
       <c r="K17" s="43"/>
     </row>
     <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" s="63" t="s">
+      <c r="A18" s="67" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="66" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E18" s="40" t="s">
         <v>25</v>
@@ -3689,13 +3896,13 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="64"/>
-      <c r="B19" s="63"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="34" t="s">
         <v>54</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E19" s="35" t="s">
         <v>25</v>
@@ -3733,17 +3940,17 @@
       <c r="K20" s="43"/>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="B21" s="63" t="s">
+      <c r="A21" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="66" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>54</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" s="40" t="s">
         <v>25</v>
@@ -3768,13 +3975,13 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
-      <c r="B22" s="63"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="34" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" s="35" t="s">
         <v>25</v>
@@ -3812,15 +4019,15 @@
       <c r="K23" s="43"/>
     </row>
     <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" s="63"/>
+      <c r="A24" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="66"/>
       <c r="C24" s="40" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E24" s="40" t="s">
         <v>25</v>
@@ -3845,13 +4052,13 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="64"/>
-      <c r="B25" s="63"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="34" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E25" s="35" t="s">
         <v>25</v>
@@ -3876,13 +4083,13 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="64"/>
-      <c r="B26" s="63"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="52" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E26" s="53" t="s">
         <v>25</v>
@@ -3921,17 +4128,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tfs6582 - ecl quality specialist coaching work flow
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C37372
</commit_message>
<xml_diff>
--- a/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
+++ b/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="132">
   <si>
     <t>CSR</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Opportunity Identified</t>
   </si>
   <si>
-    <t>Quality Specialist Coaching</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>Direct</t>
-  </si>
-  <si>
-    <t>NOT Quality Specialist Coaching</t>
   </si>
   <si>
     <t>Supervisor</t>
@@ -459,6 +453,9 @@
   </si>
   <si>
     <t>tfs6377 - ecl break feed for qs &amp; sups and other</t>
+  </si>
+  <si>
+    <t>tfs6582 - ecl quality specialist coaching work flow</t>
   </si>
 </sst>
 </file>
@@ -1156,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E17"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,16 +1169,16 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
@@ -1189,13 +1186,13 @@
         <v>41869</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="20">
         <v>1</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -1203,13 +1200,13 @@
         <v>41891</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="20">
         <v>1.1000000000000001</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -1217,13 +1214,13 @@
         <v>41905</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D5">
         <v>1.2</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -1231,13 +1228,13 @@
         <v>41908</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6">
         <v>1.3</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -1245,13 +1242,13 @@
         <v>41908</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7">
         <v>1.4</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
@@ -1259,13 +1256,13 @@
         <v>41915</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8">
         <v>1.5</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
@@ -1273,13 +1270,13 @@
         <v>41929</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D9">
         <v>1.6</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
@@ -1287,13 +1284,13 @@
         <v>41942</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D10">
         <v>1.7</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
@@ -1301,13 +1298,13 @@
         <v>41967</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D11">
         <v>1.8</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -1315,13 +1312,13 @@
         <v>42002</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D12">
         <v>1.9</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
@@ -1329,13 +1326,13 @@
         <v>42079</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D13">
         <v>1.1100000000000001</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
@@ -1343,13 +1340,13 @@
         <v>42471</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D14">
         <v>1.1200000000000001</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1357,13 +1354,13 @@
         <v>42563</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D15">
         <v>1.1299999999999999</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
@@ -1371,13 +1368,13 @@
         <v>42375</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D16">
         <v>1.1399999999999999</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
@@ -1385,13 +1382,27 @@
         <v>42845</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D17">
         <v>1.1499999999999999</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="23">
+        <v>42864</v>
+      </c>
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1401,13 +1412,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8:B12"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1427,28 +1438,28 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1471,10 +1482,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
@@ -1483,320 +1494,316 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="62" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="D8" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="E8" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="69"/>
       <c r="B9" s="70"/>
-      <c r="C9" s="52" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="52" t="s">
+      <c r="C9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="52" t="s">
+      <c r="F9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="52" t="s">
+      <c r="G9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="52" t="s">
-        <v>57</v>
+      <c r="J9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="69"/>
       <c r="B10" s="70"/>
-      <c r="C10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="C10" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="69"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="69"/>
+      <c r="B12" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="63"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="72" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="G15" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="67"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="69"/>
-      <c r="B13" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="69"/>
-      <c r="B14" s="70"/>
-      <c r="C14" s="52" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="52" t="s">
+      <c r="G16" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="52" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" s="66" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="72" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="31" t="s">
+      <c r="J16" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="K16" s="39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K16" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="67"/>
       <c r="B17" s="66"/>
       <c r="C17" s="71"/>
       <c r="D17" s="72"/>
-      <c r="E17" s="61" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="K17" s="32" t="s">
-        <v>9</v>
+      <c r="E17" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17" s="34" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -1804,398 +1811,371 @@
       <c r="B18" s="66"/>
       <c r="C18" s="71"/>
       <c r="D18" s="72"/>
-      <c r="E18" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="34" t="s">
+      <c r="E18" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="67" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="67"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="K18" s="34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="67"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="57" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="K19" s="52" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="67" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="66" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K21" s="39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="67"/>
       <c r="B22" s="66"/>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" s="52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="29"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+    </row>
+    <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="35" t="s">
+    </row>
+    <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="63"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="K25" s="55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K27" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="35" t="s">
+      <c r="H29" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K29" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="H31" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J31" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K31" s="39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J33" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K33" s="35" t="s">
         <v>54</v>
-      </c>
-      <c r="I22" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J22" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
-      <c r="B23" s="66"/>
-      <c r="C23" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" s="52" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-    </row>
-    <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="I25" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="J25" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="63"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="I26" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="J26" s="55" t="s">
-        <v>90</v>
-      </c>
-      <c r="K26" s="55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="B28" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G28" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="I28" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J28" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="F30" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="J30" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="K30" s="39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G32" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="J32" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="K32" s="39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="60" t="s">
-        <v>127</v>
-      </c>
-      <c r="B34" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="F34" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G34" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J34" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K34" s="35" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A20:A22"/>
     <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2229,33 +2209,33 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" s="36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="68" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
@@ -2273,10 +2253,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
@@ -2285,183 +2265,183 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="67" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="52" t="s">
-        <v>61</v>
-      </c>
       <c r="H8" s="52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8" s="52" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J8" s="53" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K8" s="52" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="67"/>
       <c r="B9" s="70"/>
       <c r="C9" s="40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I9" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K9" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="67"/>
       <c r="B10" s="65"/>
       <c r="C10" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="67"/>
       <c r="B11" s="66" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="34" t="s">
         <v>54</v>
-      </c>
-      <c r="I11" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="67"/>
       <c r="B12" s="66"/>
       <c r="C12" s="52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G12" s="52" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H12" s="52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I12" s="52" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J12" s="53" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K12" s="52" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2479,37 +2459,37 @@
     </row>
     <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="62" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B14" s="64" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="35" t="s">
         <v>54</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="K14" s="35" t="s">
-        <v>56</v>
       </c>
       <c r="L14" s="3"/>
     </row>
@@ -2517,102 +2497,102 @@
       <c r="A15" s="63"/>
       <c r="B15" s="65"/>
       <c r="C15" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15" s="55" t="s">
         <v>54</v>
-      </c>
-      <c r="D15" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="55" t="s">
-        <v>90</v>
-      </c>
-      <c r="K15" s="55" t="s">
-        <v>56</v>
       </c>
       <c r="L15" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B17" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="39" t="s">
-        <v>20</v>
-      </c>
       <c r="H17" s="39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I17" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="J17" s="39" t="s">
-        <v>51</v>
-      </c>
       <c r="K17" s="39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="36" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="73" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B19" s="75" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="77" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="F19" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="39" t="s">
-        <v>20</v>
-      </c>
       <c r="H19" s="39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I19" s="38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J19" s="39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K19" s="39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2621,25 +2601,25 @@
       <c r="C20" s="78"/>
       <c r="D20" s="78"/>
       <c r="E20" s="35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="35" t="s">
         <v>54</v>
-      </c>
-      <c r="I20" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="K20" s="35" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2689,30 +2669,30 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
       <c r="B2" s="36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="68" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
@@ -2730,10 +2710,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
@@ -2742,121 +2722,121 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="79" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B8" s="80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>56</v>
-      </c>
       <c r="G8" s="40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J8" s="41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K8" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="79"/>
       <c r="B9" s="81"/>
       <c r="C9" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K9" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="79"/>
       <c r="B10" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="34" t="s">
         <v>54</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2874,37 +2854,37 @@
     </row>
     <row r="12" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="35" t="s">
         <v>54</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="35" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2944,30 +2924,30 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
       <c r="B2" s="36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="68" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
@@ -2985,10 +2965,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
@@ -2997,121 +2977,121 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B8" s="80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J8" s="41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K8" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="79"/>
       <c r="B9" s="81"/>
       <c r="C9" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K9" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="79"/>
       <c r="B10" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H10" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="34" t="s">
         <v>54</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3164,13 +3144,13 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="42"/>
       <c r="B1" s="36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
       <c r="F1" s="36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G1" s="36"/>
       <c r="H1" s="36"/>
@@ -3181,13 +3161,13 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" s="36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="36"/>
       <c r="F2" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G2" s="36"/>
       <c r="H2" s="36"/>
@@ -3198,13 +3178,13 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" s="36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>
       <c r="F3" s="36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
@@ -3240,7 +3220,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="68" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
@@ -3258,10 +3238,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="37" t="s">
         <v>3</v>
@@ -3270,183 +3250,183 @@
         <v>4</v>
       </c>
       <c r="F7" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="37" t="s">
-        <v>8</v>
-      </c>
       <c r="H7" s="37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I7" s="37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K7" s="37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="79" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B8" s="80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>56</v>
-      </c>
       <c r="G8" s="40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J8" s="41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K8" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="79"/>
       <c r="B9" s="83"/>
       <c r="C9" s="52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="58" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="52" t="s">
         <v>55</v>
-      </c>
-      <c r="G9" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="H9" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9" s="52" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="79"/>
       <c r="B10" s="81"/>
       <c r="C10" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="79"/>
       <c r="B11" s="82" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="34" t="s">
         <v>54</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="79"/>
       <c r="B12" s="82"/>
       <c r="C12" s="52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="52" t="s">
         <v>55</v>
-      </c>
-      <c r="G12" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="H12" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="K12" s="52" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3504,28 +3484,28 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="42"/>
       <c r="B1" s="36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" s="36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" s="36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3548,10 +3528,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="37" t="s">
         <v>3</v>
@@ -3560,150 +3540,150 @@
         <v>4</v>
       </c>
       <c r="F7" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="37" t="s">
-        <v>8</v>
-      </c>
       <c r="H7" s="37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I7" s="37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K7" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="67" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B8" s="66" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H8" s="39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="39" t="s">
-        <v>51</v>
-      </c>
       <c r="K8" s="39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="67"/>
       <c r="B9" s="66"/>
       <c r="C9" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>56</v>
-      </c>
       <c r="G9" s="40" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I9" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K9" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="67"/>
       <c r="B10" s="66"/>
       <c r="C10" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="34" t="s">
         <v>54</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="67"/>
       <c r="B11" s="66"/>
       <c r="C11" s="52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="52" t="s">
         <v>55</v>
-      </c>
-      <c r="G11" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="52" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3721,130 +3701,130 @@
     </row>
     <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="67" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B13" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>20</v>
-      </c>
       <c r="H13" s="39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I13" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="39" t="s">
-        <v>51</v>
-      </c>
       <c r="K13" s="39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="67"/>
       <c r="B14" s="66"/>
       <c r="C14" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>56</v>
-      </c>
       <c r="G14" s="40" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I14" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J14" s="41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K14" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="67"/>
       <c r="B15" s="66"/>
       <c r="C15" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="34" t="s">
         <v>54</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="67"/>
       <c r="B16" s="66"/>
       <c r="C16" s="52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E16" s="53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16" s="52" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G16" s="52" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H16" s="52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I16" s="52" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J16" s="53" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K16" s="52" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -3862,68 +3842,68 @@
     </row>
     <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="67" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B18" s="66" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="40" t="s">
-        <v>56</v>
-      </c>
       <c r="G18" s="40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H18" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I18" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J18" s="41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K18" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="67"/>
       <c r="B19" s="66"/>
       <c r="C19" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="34" t="s">
         <v>54</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="J19" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -3941,68 +3921,68 @@
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B21" s="66" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="40" t="s">
-        <v>56</v>
-      </c>
       <c r="G21" s="40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H21" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I21" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J21" s="41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K21" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="67"/>
       <c r="B22" s="66"/>
       <c r="C22" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K22" s="34" t="s">
         <v>54</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="H22" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J22" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -4020,97 +4000,97 @@
     </row>
     <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="67" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B24" s="66"/>
       <c r="C24" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>56</v>
-      </c>
       <c r="G24" s="40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H24" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I24" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J24" s="41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K24" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="67"/>
       <c r="B25" s="66"/>
       <c r="C25" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K25" s="34" t="s">
         <v>54</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="H25" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="I25" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="J25" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="34" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="67"/>
       <c r="B26" s="66"/>
       <c r="C26" s="52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E26" s="53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F26" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="H26" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="52" t="s">
         <v>55</v>
-      </c>
-      <c r="G26" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="H26" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="I26" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="J26" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="K26" s="52" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -4128,17 +4108,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="A6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tfs7174 - ecl new ets feeds
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C38285
</commit_message>
<xml_diff>
--- a/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
+++ b/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="133">
   <si>
     <t>CSR</t>
   </si>
@@ -304,16 +304,6 @@
 Research Required</t>
   </si>
   <si>
-    <t>ETS
-(EA,HOL,ITD,ITI,FWH)
-Opportunity</t>
-  </si>
-  <si>
-    <t>ETS
-(EOT,EA,HOLA,ITDA,ITIA,FWHA)
-Opportunity</t>
-  </si>
-  <si>
     <t>Training</t>
   </si>
   <si>
@@ -456,6 +446,20 @@
   </si>
   <si>
     <t>tfs6582 - ecl quality specialist coaching work flow</t>
+  </si>
+  <si>
+    <t>ETS
+(EA,HOL,ITD,ITI,FWH,HNC,ICC)
+Opportunity</t>
+  </si>
+  <si>
+    <t>tfs7174 - ecl new ets feeds</t>
+  </si>
+  <si>
+    <t>ETS
+(EA,HOL,ITD,ITI,FWH)
+(EOT,HOLA,ITDA,ITIA,FWHA)
+Opportunity</t>
   </si>
 </sst>
 </file>
@@ -799,17 +803,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1153,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E18"/>
+  <dimension ref="B2:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,7 +1330,7 @@
         <v>42079</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D13">
         <v>1.1100000000000001</v>
@@ -1340,7 +1344,7 @@
         <v>42471</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D14">
         <v>1.1200000000000001</v>
@@ -1354,7 +1358,7 @@
         <v>42563</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D15">
         <v>1.1299999999999999</v>
@@ -1368,7 +1372,7 @@
         <v>42375</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D16">
         <v>1.1399999999999999</v>
@@ -1382,7 +1386,7 @@
         <v>42845</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D17">
         <v>1.1499999999999999</v>
@@ -1396,12 +1400,26 @@
         <v>42864</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D18">
         <v>1.1599999999999999</v>
       </c>
       <c r="E18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="23">
+        <v>42942</v>
+      </c>
+      <c r="C19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19">
+        <v>1.17</v>
+      </c>
+      <c r="E19" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1418,7 +1436,7 @@
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:A13"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1548,8 +1566,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="69"/>
-      <c r="B9" s="70"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
@@ -1579,8 +1597,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="69"/>
-      <c r="B10" s="70"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="40" t="s">
         <v>5</v>
       </c>
@@ -1610,7 +1628,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
+      <c r="A11" s="72"/>
       <c r="B11" s="65"/>
       <c r="C11" s="25" t="s">
         <v>9</v>
@@ -1641,7 +1659,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="64" t="s">
         <v>16</v>
       </c>
@@ -1675,7 +1693,7 @@
     </row>
     <row r="13" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="63"/>
-      <c r="B13" s="70"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="52" t="s">
         <v>5</v>
       </c>
@@ -1719,19 +1737,19 @@
     </row>
     <row r="15" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="67" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B15" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="72" t="s">
+      <c r="C15" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="71" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F15" s="30" t="s">
         <v>56</v>
@@ -1749,16 +1767,16 @@
         <v>81</v>
       </c>
       <c r="K15" s="39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="67"/>
       <c r="B16" s="66"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="72"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="71"/>
       <c r="E16" s="61" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>54</v>
@@ -1782,10 +1800,10 @@
     <row r="17" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="67"/>
       <c r="B17" s="66"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="72"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="71"/>
       <c r="E17" s="46" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>55</v>
@@ -1809,10 +1827,10 @@
     <row r="18" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="67"/>
       <c r="B18" s="66"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="72"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="57" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F18" s="52" t="s">
         <v>53</v>
@@ -1848,7 +1866,7 @@
     </row>
     <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="67" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B20" s="66" t="s">
         <v>16</v>
@@ -1878,7 +1896,7 @@
         <v>49</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1919,7 +1937,7 @@
         <v>52</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E22" s="53" t="s">
         <v>25</v>
@@ -1958,7 +1976,7 @@
     </row>
     <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="62" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B24" s="64" t="s">
         <v>16</v>
@@ -1970,7 +1988,7 @@
         <v>52</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="F24" s="35" t="s">
         <v>55</v>
@@ -2024,7 +2042,7 @@
     </row>
     <row r="27" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B27" s="44" t="s">
         <v>16</v>
@@ -2036,7 +2054,7 @@
         <v>26</v>
       </c>
       <c r="E27" s="35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F27" s="34" t="s">
         <v>55</v>
@@ -2059,7 +2077,7 @@
     </row>
     <row r="29" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B29" s="44" t="s">
         <v>16</v>
@@ -2071,7 +2089,7 @@
         <v>26</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F29" s="38" t="s">
         <v>56</v>
@@ -2089,12 +2107,12 @@
         <v>49</v>
       </c>
       <c r="K29" s="39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B31" s="47" t="s">
         <v>16</v>
@@ -2106,7 +2124,7 @@
         <v>5</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F31" s="38" t="s">
         <v>56</v>
@@ -2124,12 +2142,12 @@
         <v>49</v>
       </c>
       <c r="K31" s="39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="60" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B33" s="59" t="s">
         <v>16</v>
@@ -2141,7 +2159,7 @@
         <v>5</v>
       </c>
       <c r="E33" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F33" s="34" t="s">
         <v>55</v>
@@ -2320,7 +2338,7 @@
     </row>
     <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="67"/>
-      <c r="B9" s="70"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="40" t="s">
         <v>5</v>
       </c>
@@ -2459,7 +2477,7 @@
     </row>
     <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="62" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B14" s="64" t="s">
         <v>16</v>
@@ -2471,7 +2489,7 @@
         <v>52</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>58</v>
@@ -2527,7 +2545,7 @@
     </row>
     <row r="17" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B17" s="47" t="s">
         <v>16</v>
@@ -2539,7 +2557,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F17" s="38" t="s">
         <v>56</v>
@@ -2557,12 +2575,12 @@
         <v>49</v>
       </c>
       <c r="K17" s="39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="36" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="73" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B19" s="75" t="s">
         <v>16</v>
@@ -2574,7 +2592,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F19" s="38" t="s">
         <v>56</v>
@@ -2592,7 +2610,7 @@
         <v>81</v>
       </c>
       <c r="K19" s="39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2601,7 +2619,7 @@
       <c r="C20" s="78"/>
       <c r="D20" s="78"/>
       <c r="E20" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F20" s="34" t="s">
         <v>58</v>
@@ -2854,7 +2872,7 @@
     </row>
     <row r="12" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B12" s="59" t="s">
         <v>16</v>
@@ -2866,7 +2884,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>60</v>
@@ -3220,7 +3238,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="68" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
@@ -3270,7 +3288,7 @@
     </row>
     <row r="8" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="79" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="80" t="s">
         <v>14</v>
@@ -3288,7 +3306,7 @@
         <v>54</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H8" s="40" t="s">
         <v>52</v>
@@ -3319,7 +3337,7 @@
         <v>53</v>
       </c>
       <c r="G9" s="52" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H9" s="52" t="s">
         <v>52</v>
@@ -3383,7 +3401,7 @@
         <v>55</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H11" s="34" t="s">
         <v>52</v>
@@ -3414,7 +3432,7 @@
         <v>53</v>
       </c>
       <c r="G12" s="52" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H12" s="52" t="s">
         <v>52</v>
@@ -3560,7 +3578,7 @@
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="67" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B8" s="66" t="s">
         <v>16</v>
@@ -3569,7 +3587,7 @@
         <v>52</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>23</v>
@@ -3590,7 +3608,7 @@
         <v>49</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -3600,7 +3618,7 @@
         <v>52</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E9" s="40" t="s">
         <v>23</v>
@@ -3631,7 +3649,7 @@
         <v>52</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>23</v>
@@ -3662,7 +3680,7 @@
         <v>52</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E11" s="53" t="s">
         <v>23</v>
@@ -3701,7 +3719,7 @@
     </row>
     <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="67" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B13" s="66" t="s">
         <v>16</v>
@@ -3710,7 +3728,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E13" s="39" t="s">
         <v>23</v>
@@ -3731,7 +3749,7 @@
         <v>49</v>
       </c>
       <c r="K13" s="39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -3741,7 +3759,7 @@
         <v>52</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E14" s="40" t="s">
         <v>23</v>
@@ -3772,7 +3790,7 @@
         <v>52</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>23</v>
@@ -3803,7 +3821,7 @@
         <v>52</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E16" s="53" t="s">
         <v>23</v>
@@ -3842,7 +3860,7 @@
     </row>
     <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="67" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B18" s="66" t="s">
         <v>16</v>
@@ -3851,7 +3869,7 @@
         <v>52</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E18" s="40" t="s">
         <v>23</v>
@@ -3882,7 +3900,7 @@
         <v>52</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E19" s="35" t="s">
         <v>23</v>
@@ -3921,7 +3939,7 @@
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B21" s="66" t="s">
         <v>16</v>
@@ -3930,7 +3948,7 @@
         <v>52</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E21" s="40" t="s">
         <v>23</v>
@@ -3961,7 +3979,7 @@
         <v>52</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E22" s="35" t="s">
         <v>23</v>
@@ -4000,14 +4018,14 @@
     </row>
     <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="67" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B24" s="66"/>
       <c r="C24" s="40" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E24" s="40" t="s">
         <v>23</v>
@@ -4016,7 +4034,7 @@
         <v>54</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H24" s="40" t="s">
         <v>52</v>
@@ -4038,7 +4056,7 @@
         <v>52</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E25" s="35" t="s">
         <v>23</v>
@@ -4047,7 +4065,7 @@
         <v>55</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H25" s="35" t="s">
         <v>52</v>
@@ -4069,7 +4087,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E26" s="53" t="s">
         <v>23</v>
@@ -4078,7 +4096,7 @@
         <v>53</v>
       </c>
       <c r="G26" s="52" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H26" s="52" t="s">
         <v>52</v>
@@ -4108,17 +4126,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tfs7646 - ecl discrepancy feed
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C38482
</commit_message>
<xml_diff>
--- a/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
+++ b/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="136">
   <si>
     <t>CSR</t>
   </si>
@@ -460,6 +460,17 @@
 (EA,HOL,ITD,ITI,FWH)
 (EOT,HOLA,ITDA,ITIA,FWHA)
 Opportunity</t>
+  </si>
+  <si>
+    <t>Generic DTT data feed</t>
+  </si>
+  <si>
+    <t>Empower
+(OTH_DTT)
+Opportunity</t>
+  </si>
+  <si>
+    <t>tfs7646 - ecl discrepancy feed</t>
   </si>
 </sst>
 </file>
@@ -641,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -781,6 +792,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1157,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1423,6 +1440,20 @@
         <v>70</v>
       </c>
     </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="23">
+        <v>42971</v>
+      </c>
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20">
+        <v>1.18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1433,10 +1464,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8:B11"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1481,19 +1512,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1531,10 +1562,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="66" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="52" t="s">
@@ -1566,8 +1597,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="72"/>
-      <c r="B9" s="69"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
@@ -1597,8 +1628,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="72"/>
-      <c r="B10" s="69"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="40" t="s">
         <v>5</v>
       </c>
@@ -1628,8 +1659,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="72"/>
-      <c r="B11" s="65"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="25" t="s">
         <v>9</v>
       </c>
@@ -1659,8 +1690,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="72"/>
-      <c r="B12" s="64" t="s">
+      <c r="A12" s="74"/>
+      <c r="B12" s="66" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="34" t="s">
@@ -1692,8 +1723,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="63"/>
-      <c r="B13" s="69"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="71"/>
       <c r="C13" s="52" t="s">
         <v>5</v>
       </c>
@@ -1736,16 +1767,16 @@
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="71" t="s">
+      <c r="C15" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="73" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="39" t="s">
@@ -1771,10 +1802,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="71"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="61" t="s">
         <v>97</v>
       </c>
@@ -1798,10 +1829,10 @@
       </c>
     </row>
     <row r="17" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="67"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="71"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="73"/>
       <c r="E17" s="46" t="s">
         <v>122</v>
       </c>
@@ -1825,10 +1856,10 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="67"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="71"/>
+      <c r="A18" s="69"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="73"/>
       <c r="E18" s="57" t="s">
         <v>98</v>
       </c>
@@ -1865,10 +1896,10 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="69" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="68" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1900,8 +1931,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
-      <c r="B21" s="66"/>
+      <c r="A21" s="69"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="34" t="s">
         <v>52</v>
       </c>
@@ -1931,8 +1962,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A22" s="67"/>
-      <c r="B22" s="66"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="68"/>
       <c r="C22" s="52" t="s">
         <v>52</v>
       </c>
@@ -1975,10 +2006,10 @@
       <c r="K23" s="14"/>
     </row>
     <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="62" t="s">
+      <c r="A24" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="66" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="34" t="s">
@@ -2010,8 +2041,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="65"/>
+      <c r="A25" s="65"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="54" t="s">
         <v>52</v>
       </c>
@@ -2202,13 +2233,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8:B10"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2252,19 +2283,19 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2302,10 +2333,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="66" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="52" t="s">
@@ -2337,8 +2368,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="67"/>
-      <c r="B9" s="69"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="40" t="s">
         <v>5</v>
       </c>
@@ -2368,8 +2399,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="67"/>
-      <c r="B10" s="65"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="25" t="s">
         <v>9</v>
       </c>
@@ -2399,8 +2430,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
-      <c r="B11" s="66" t="s">
+      <c r="A11" s="69"/>
+      <c r="B11" s="68" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -2432,8 +2463,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="66"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="52" t="s">
         <v>5</v>
       </c>
@@ -2476,10 +2507,10 @@
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="66" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="34" t="s">
@@ -2512,8 +2543,8 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="63"/>
-      <c r="B15" s="65"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="54" t="s">
         <v>52</v>
       </c>
@@ -2579,16 +2610,16 @@
       </c>
     </row>
     <row r="19" spans="1:11" s="36" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="77" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="77" t="s">
+      <c r="C19" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="79" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="39" t="s">
@@ -2614,10 +2645,10 @@
       </c>
     </row>
     <row r="20" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="74"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
+      <c r="A20" s="76"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
       <c r="E20" s="35" t="s">
         <v>127</v>
       </c>
@@ -2638,6 +2669,41 @@
       </c>
       <c r="K20" s="35" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="36" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J22" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22" s="39" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2709,19 +2775,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2759,10 +2825,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="82" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -2794,8 +2860,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="79"/>
-      <c r="B9" s="81"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="25" t="s">
         <v>9</v>
       </c>
@@ -2825,7 +2891,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
+      <c r="A10" s="81"/>
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
@@ -2964,19 +3030,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -3014,10 +3080,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="82" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -3049,8 +3115,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="79"/>
-      <c r="B9" s="81"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="25" t="s">
         <v>9</v>
       </c>
@@ -3080,7 +3146,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
+      <c r="A10" s="81"/>
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
@@ -3237,19 +3303,19 @@
       <c r="K5" s="36"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
@@ -3287,10 +3353,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="82" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -3322,8 +3388,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="79"/>
-      <c r="B9" s="83"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="52" t="s">
         <v>52</v>
       </c>
@@ -3353,8 +3419,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
-      <c r="B10" s="81"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="25" t="s">
         <v>9</v>
       </c>
@@ -3384,8 +3450,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="79"/>
-      <c r="B11" s="82" t="s">
+      <c r="A11" s="81"/>
+      <c r="B11" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -3417,8 +3483,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="79"/>
-      <c r="B12" s="82"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="84"/>
       <c r="C12" s="52" t="s">
         <v>52</v>
       </c>
@@ -3527,19 +3593,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
@@ -3577,10 +3643,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="68" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="38" t="s">
@@ -3612,8 +3678,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="67"/>
-      <c r="B9" s="66"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="40" t="s">
         <v>52</v>
       </c>
@@ -3643,8 +3709,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="67"/>
-      <c r="B10" s="66"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="34" t="s">
         <v>52</v>
       </c>
@@ -3674,8 +3740,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
-      <c r="B11" s="66"/>
+      <c r="A11" s="69"/>
+      <c r="B11" s="68"/>
       <c r="C11" s="52" t="s">
         <v>52</v>
       </c>
@@ -3718,10 +3784,10 @@
       <c r="K12" s="43"/>
     </row>
     <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="68" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -3753,8 +3819,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="67"/>
-      <c r="B14" s="66"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="40" t="s">
         <v>52</v>
       </c>
@@ -3784,8 +3850,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="67"/>
-      <c r="B15" s="66"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="68"/>
       <c r="C15" s="34" t="s">
         <v>52</v>
       </c>
@@ -3815,8 +3881,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
-      <c r="B16" s="66"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="52" t="s">
         <v>52</v>
       </c>
@@ -3859,10 +3925,10 @@
       <c r="K17" s="43"/>
     </row>
     <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="67" t="s">
+      <c r="A18" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="68" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="40" t="s">
@@ -3894,8 +3960,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="67"/>
-      <c r="B19" s="66"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="34" t="s">
         <v>52</v>
       </c>
@@ -3938,10 +4004,10 @@
       <c r="K20" s="43"/>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="67" t="s">
+      <c r="A21" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="68" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -3973,8 +4039,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="67"/>
-      <c r="B22" s="66"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="68"/>
       <c r="C22" s="34" t="s">
         <v>52</v>
       </c>
@@ -4017,10 +4083,10 @@
       <c r="K23" s="43"/>
     </row>
     <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="66"/>
+      <c r="B24" s="68"/>
       <c r="C24" s="40" t="s">
         <v>52</v>
       </c>
@@ -4050,8 +4116,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="67"/>
-      <c r="B25" s="66"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="34" t="s">
         <v>52</v>
       </c>
@@ -4081,8 +4147,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="67"/>
-      <c r="B26" s="66"/>
+      <c r="A26" s="69"/>
+      <c r="B26" s="68"/>
       <c r="C26" s="52" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
tfs7541 - ecl ata forms from iqs
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C38558
</commit_message>
<xml_diff>
--- a/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
+++ b/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18192" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18192" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="139">
   <si>
     <t>CSR</t>
   </si>
@@ -471,6 +471,16 @@
   </si>
   <si>
     <t>tfs7646 - ecl discrepancy feed</t>
+  </si>
+  <si>
+    <t>Completed
+(Pending Employee Review - Level 1 or Pending Quality Lead Review - Level 2)</t>
+  </si>
+  <si>
+    <t>IQS data feed (ATA)</t>
+  </si>
+  <si>
+    <t>tfs7541 - ecl ata feed from iqs</t>
   </si>
 </sst>
 </file>
@@ -652,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -792,6 +802,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1174,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E20"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1454,6 +1470,20 @@
         <v>70</v>
       </c>
     </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="23">
+        <v>42984</v>
+      </c>
+      <c r="C21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21">
+        <v>1.19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1463,11 +1493,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1512,19 +1542,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1562,10 +1592,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="68" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="52" t="s">
@@ -1597,8 +1627,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="74"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
@@ -1628,8 +1658,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="74"/>
-      <c r="B10" s="71"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="40" t="s">
         <v>5</v>
       </c>
@@ -1659,8 +1689,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="74"/>
-      <c r="B11" s="67"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="25" t="s">
         <v>9</v>
       </c>
@@ -1690,8 +1720,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="74"/>
-      <c r="B12" s="66" t="s">
+      <c r="A12" s="76"/>
+      <c r="B12" s="68" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="34" t="s">
@@ -1723,8 +1753,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="65"/>
-      <c r="B13" s="71"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="73"/>
       <c r="C13" s="52" t="s">
         <v>5</v>
       </c>
@@ -1767,16 +1797,16 @@
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="73" t="s">
+      <c r="C15" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="75" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="39" t="s">
@@ -1802,10 +1832,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="69"/>
-      <c r="B16" s="68"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="73"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="75"/>
       <c r="E16" s="61" t="s">
         <v>97</v>
       </c>
@@ -1829,10 +1859,10 @@
       </c>
     </row>
     <row r="17" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="69"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="73"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="75"/>
       <c r="E17" s="46" t="s">
         <v>122</v>
       </c>
@@ -1856,10 +1886,10 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="69"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="73"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="75"/>
       <c r="E18" s="57" t="s">
         <v>98</v>
       </c>
@@ -1896,10 +1926,10 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="70" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1931,8 +1961,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="69"/>
-      <c r="B21" s="68"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="70"/>
       <c r="C21" s="34" t="s">
         <v>52</v>
       </c>
@@ -1962,8 +1992,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A22" s="69"/>
-      <c r="B22" s="68"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="70"/>
       <c r="C22" s="52" t="s">
         <v>52</v>
       </c>
@@ -2006,10 +2036,10 @@
       <c r="K23" s="14"/>
     </row>
     <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="68" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="34" t="s">
@@ -2041,8 +2071,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
-      <c r="B25" s="67"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="69"/>
       <c r="C25" s="54" t="s">
         <v>52</v>
       </c>
@@ -2236,10 +2266,10 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2283,19 +2313,19 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2333,10 +2363,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="68" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="52" t="s">
@@ -2368,8 +2398,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="69"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="40" t="s">
         <v>5</v>
       </c>
@@ -2399,8 +2429,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="69"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="25" t="s">
         <v>9</v>
       </c>
@@ -2430,8 +2460,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
-      <c r="B11" s="68" t="s">
+      <c r="A11" s="71"/>
+      <c r="B11" s="70" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -2463,8 +2493,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
-      <c r="B12" s="68"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="52" t="s">
         <v>5</v>
       </c>
@@ -2507,10 +2537,10 @@
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="68" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="34" t="s">
@@ -2543,8 +2573,8 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="65"/>
-      <c r="B15" s="67"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="69"/>
       <c r="C15" s="54" t="s">
         <v>52</v>
       </c>
@@ -2610,16 +2640,16 @@
       </c>
     </row>
     <row r="19" spans="1:11" s="36" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="75" t="s">
+      <c r="A19" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="79" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="79" t="s">
+      <c r="C19" s="81" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="81" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="39" t="s">
@@ -2645,10 +2675,10 @@
       </c>
     </row>
     <row r="20" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="76"/>
-      <c r="B20" s="78"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
       <c r="E20" s="35" t="s">
         <v>127</v>
       </c>
@@ -2726,13 +2756,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2775,19 +2805,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2825,10 +2855,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="84" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -2860,8 +2890,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="81"/>
-      <c r="B9" s="83"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="25" t="s">
         <v>9</v>
       </c>
@@ -2891,7 +2921,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="81"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
@@ -2969,6 +2999,41 @@
       </c>
       <c r="K12" s="35" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="39" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3030,19 +3095,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -3080,10 +3145,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="84" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -3115,8 +3180,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="81"/>
-      <c r="B9" s="83"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="25" t="s">
         <v>9</v>
       </c>
@@ -3146,7 +3211,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="81"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
@@ -3303,19 +3368,19 @@
       <c r="K5" s="36"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
@@ -3353,10 +3418,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="84" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -3388,8 +3453,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="81"/>
-      <c r="B9" s="85"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="87"/>
       <c r="C9" s="52" t="s">
         <v>52</v>
       </c>
@@ -3419,8 +3484,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="81"/>
-      <c r="B10" s="83"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="85"/>
       <c r="C10" s="25" t="s">
         <v>9</v>
       </c>
@@ -3450,8 +3515,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="81"/>
-      <c r="B11" s="84" t="s">
+      <c r="A11" s="83"/>
+      <c r="B11" s="86" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -3483,8 +3548,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="81"/>
-      <c r="B12" s="84"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="52" t="s">
         <v>52</v>
       </c>
@@ -3593,19 +3658,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
@@ -3643,10 +3708,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="70" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="38" t="s">
@@ -3678,8 +3743,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="69"/>
-      <c r="B9" s="68"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="40" t="s">
         <v>52</v>
       </c>
@@ -3709,8 +3774,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="69"/>
-      <c r="B10" s="68"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="70"/>
       <c r="C10" s="34" t="s">
         <v>52</v>
       </c>
@@ -3740,8 +3805,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
-      <c r="B11" s="68"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="52" t="s">
         <v>52</v>
       </c>
@@ -3784,10 +3849,10 @@
       <c r="K12" s="43"/>
     </row>
     <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="70" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -3819,8 +3884,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="69"/>
-      <c r="B14" s="68"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="40" t="s">
         <v>52</v>
       </c>
@@ -3850,8 +3915,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="69"/>
-      <c r="B15" s="68"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="34" t="s">
         <v>52</v>
       </c>
@@ -3881,8 +3946,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="69"/>
-      <c r="B16" s="68"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="52" t="s">
         <v>52</v>
       </c>
@@ -3925,10 +3990,10 @@
       <c r="K17" s="43"/>
     </row>
     <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="69" t="s">
+      <c r="A18" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="70" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="40" t="s">
@@ -3960,8 +4025,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="69"/>
-      <c r="B19" s="68"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="70"/>
       <c r="C19" s="34" t="s">
         <v>52</v>
       </c>
@@ -4004,10 +4069,10 @@
       <c r="K20" s="43"/>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="69" t="s">
+      <c r="A21" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="70" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -4039,8 +4104,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="69"/>
-      <c r="B22" s="68"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="70"/>
       <c r="C22" s="34" t="s">
         <v>52</v>
       </c>
@@ -4083,10 +4148,10 @@
       <c r="K23" s="43"/>
     </row>
     <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="69" t="s">
+      <c r="A24" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="68"/>
+      <c r="B24" s="70"/>
       <c r="C24" s="40" t="s">
         <v>52</v>
       </c>
@@ -4116,8 +4181,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="69"/>
-      <c r="B25" s="68"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="70"/>
       <c r="C25" s="34" t="s">
         <v>52</v>
       </c>
@@ -4147,8 +4212,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="69"/>
-      <c r="B26" s="68"/>
+      <c r="A26" s="71"/>
+      <c r="B26" s="70"/>
       <c r="C26" s="52" t="s">
         <v>52</v>
       </c>
@@ -4192,17 +4257,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="A6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tfs8597 - ecl dtt feed changes
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C38813
</commit_message>
<xml_diff>
--- a/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
+++ b/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18192" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18192" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="140">
   <si>
     <t>CSR</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>tfs7541 - ecl ata feed from iqs</t>
+  </si>
+  <si>
+    <t>tfs8597 - ecl dtt feed changes (sup tab line 22)</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -649,20 +652,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -848,24 +842,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -880,6 +856,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1190,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E21"/>
+  <dimension ref="B2:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1481,6 +1460,20 @@
         <v>1.19</v>
       </c>
       <c r="E21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="23">
+        <v>43020</v>
+      </c>
+      <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22">
+        <v>1.2</v>
+      </c>
+      <c r="E22" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2265,11 +2258,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8:B10"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2640,16 +2633,16 @@
       </c>
     </row>
     <row r="19" spans="1:11" s="36" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="81" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="81" t="s">
+      <c r="C19" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="82" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="39" t="s">
@@ -2675,8 +2668,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="78"/>
-      <c r="B20" s="80"/>
+      <c r="A20" s="71"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="82"/>
       <c r="D20" s="82"/>
       <c r="E20" s="35" t="s">
@@ -2701,7 +2694,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="36" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="63" t="s">
         <v>133</v>
       </c>
@@ -2718,22 +2711,22 @@
         <v>134</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G22" s="39" t="s">
         <v>18</v>
       </c>
       <c r="H22" s="39" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="I22" s="38" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J22" s="39" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="K22" s="39" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2758,7 +2751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -2855,10 +2848,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="78" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -2890,8 +2883,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="85"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="25" t="s">
         <v>9</v>
       </c>
@@ -2921,7 +2914,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="83"/>
+      <c r="A10" s="77"/>
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
@@ -3145,10 +3138,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="78" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -3180,8 +3173,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="85"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="25" t="s">
         <v>9</v>
       </c>
@@ -3211,7 +3204,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="83"/>
+      <c r="A10" s="77"/>
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
@@ -3418,10 +3411,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="78" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -3453,8 +3446,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="87"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="52" t="s">
         <v>52</v>
       </c>
@@ -3484,8 +3477,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="83"/>
-      <c r="B10" s="85"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="25" t="s">
         <v>9</v>
       </c>
@@ -3515,8 +3508,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="83"/>
-      <c r="B11" s="86" t="s">
+      <c r="A11" s="77"/>
+      <c r="B11" s="80" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -3548,8 +3541,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="83"/>
-      <c r="B12" s="86"/>
+      <c r="A12" s="77"/>
+      <c r="B12" s="80"/>
       <c r="C12" s="52" t="s">
         <v>52</v>
       </c>
@@ -4257,17 +4250,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tfs8747 - ecl update for ets email text
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C38843
</commit_message>
<xml_diff>
--- a/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
+++ b/Requirements/Misc/CCO_eCL_Status_Email_Notify.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18192" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18192" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="140">
   <si>
     <t>CSR</t>
   </si>
@@ -289,9 +289,6 @@
   </si>
   <si>
     <t>P14031 - eCL ETS Non-compliance report</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A new eCoaching Log has been entered and requires your action. Please click on the link below to review and verify that the eCL entered on &lt;DATE&gt; for &lt;EMPLOYEE NAME&gt; is a valid timecard infraction. Further directions are provided on the form. </t>
   </si>
   <si>
     <t>ETS
@@ -484,6 +481,9 @@
   </si>
   <si>
     <t>tfs8597 - ecl dtt feed changes (sup tab line 22)</t>
+  </si>
+  <si>
+    <t>tfs8747 - ecl ets email text (csr tab line 25 and supervisor tab, line 15)</t>
   </si>
 </sst>
 </file>
@@ -843,6 +843,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -856,9 +859,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1169,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1342,7 +1342,7 @@
         <v>42079</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13">
         <v>1.1100000000000001</v>
@@ -1356,7 +1356,7 @@
         <v>42471</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14">
         <v>1.1200000000000001</v>
@@ -1370,7 +1370,7 @@
         <v>42563</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D15">
         <v>1.1299999999999999</v>
@@ -1384,7 +1384,7 @@
         <v>42375</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D16">
         <v>1.1399999999999999</v>
@@ -1398,7 +1398,7 @@
         <v>42845</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D17">
         <v>1.1499999999999999</v>
@@ -1412,7 +1412,7 @@
         <v>42864</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D18">
         <v>1.1599999999999999</v>
@@ -1426,7 +1426,7 @@
         <v>42942</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D19">
         <v>1.17</v>
@@ -1440,7 +1440,7 @@
         <v>42971</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D20">
         <v>1.18</v>
@@ -1454,7 +1454,7 @@
         <v>42984</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D21">
         <v>1.19</v>
@@ -1468,12 +1468,26 @@
         <v>43020</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D22">
         <v>1.2</v>
       </c>
       <c r="E22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="23">
+        <v>43025</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23">
+        <v>1.21</v>
+      </c>
+      <c r="E23" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1487,10 +1501,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8:B11"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1503,7 +1517,7 @@
     <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="61" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.109375" customWidth="1"/>
+    <col min="10" max="10" width="57.21875" customWidth="1"/>
     <col min="11" max="11" width="33.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1619,7 +1633,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="76"/>
       <c r="B9" s="73"/>
       <c r="C9" s="6" t="s">
@@ -1650,7 +1664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="76"/>
       <c r="B10" s="73"/>
       <c r="C10" s="40" t="s">
@@ -1745,7 +1759,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="67"/>
       <c r="B13" s="73"/>
       <c r="C13" s="52" t="s">
@@ -1791,7 +1805,7 @@
     </row>
     <row r="15" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="70" t="s">
         <v>16</v>
@@ -1803,7 +1817,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F15" s="30" t="s">
         <v>56</v>
@@ -1821,7 +1835,7 @@
         <v>81</v>
       </c>
       <c r="K15" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -1830,7 +1844,7 @@
       <c r="C16" s="74"/>
       <c r="D16" s="75"/>
       <c r="E16" s="61" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>54</v>
@@ -1857,7 +1871,7 @@
       <c r="C17" s="74"/>
       <c r="D17" s="75"/>
       <c r="E17" s="46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>55</v>
@@ -1884,7 +1898,7 @@
       <c r="C18" s="74"/>
       <c r="D18" s="75"/>
       <c r="E18" s="57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F18" s="52" t="s">
         <v>53</v>
@@ -1920,7 +1934,7 @@
     </row>
     <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="70" t="s">
         <v>16</v>
@@ -1950,10 +1964,10 @@
         <v>49</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="71"/>
       <c r="B21" s="70"/>
       <c r="C21" s="34" t="s">
@@ -1991,7 +2005,7 @@
         <v>52</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E22" s="53" t="s">
         <v>25</v>
@@ -2028,9 +2042,9 @@
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
     </row>
-    <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="68" t="s">
         <v>16</v>
@@ -2042,7 +2056,7 @@
         <v>52</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F24" s="35" t="s">
         <v>55</v>
@@ -2063,7 +2077,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="67"/>
       <c r="B25" s="69"/>
       <c r="C25" s="54" t="s">
@@ -2073,7 +2087,7 @@
         <v>52</v>
       </c>
       <c r="E25" s="55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F25" s="55" t="s">
         <v>55</v>
@@ -2088,15 +2102,15 @@
         <v>31</v>
       </c>
       <c r="J25" s="55" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="K25" s="55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" s="36" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="44" t="s">
         <v>16</v>
@@ -2108,7 +2122,7 @@
         <v>26</v>
       </c>
       <c r="E27" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F27" s="34" t="s">
         <v>55</v>
@@ -2131,7 +2145,7 @@
     </row>
     <row r="29" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B29" s="44" t="s">
         <v>16</v>
@@ -2143,7 +2157,7 @@
         <v>26</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F29" s="38" t="s">
         <v>56</v>
@@ -2161,12 +2175,12 @@
         <v>49</v>
       </c>
       <c r="K29" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31" s="47" t="s">
         <v>16</v>
@@ -2178,7 +2192,7 @@
         <v>5</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F31" s="38" t="s">
         <v>56</v>
@@ -2196,12 +2210,12 @@
         <v>49</v>
       </c>
       <c r="K31" s="39" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="36" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="59" t="s">
         <v>16</v>
@@ -2213,7 +2227,7 @@
         <v>5</v>
       </c>
       <c r="E33" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F33" s="34" t="s">
         <v>55</v>
@@ -2258,11 +2272,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2531,7 +2545,7 @@
     </row>
     <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="68" t="s">
         <v>16</v>
@@ -2543,7 +2557,7 @@
         <v>52</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>58</v>
@@ -2565,7 +2579,7 @@
       </c>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="67"/>
       <c r="B15" s="69"/>
       <c r="C15" s="54" t="s">
@@ -2575,7 +2589,7 @@
         <v>52</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" s="55" t="s">
         <v>58</v>
@@ -2590,7 +2604,7 @@
         <v>30</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="K15" s="55" t="s">
         <v>54</v>
@@ -2599,7 +2613,7 @@
     </row>
     <row r="17" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="47" t="s">
         <v>16</v>
@@ -2611,7 +2625,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F17" s="38" t="s">
         <v>56</v>
@@ -2629,24 +2643,24 @@
         <v>49</v>
       </c>
       <c r="K17" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="36" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="82" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="82" t="s">
+      <c r="C19" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="77" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F19" s="38" t="s">
         <v>56</v>
@@ -2664,16 +2678,16 @@
         <v>81</v>
       </c>
       <c r="K19" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="71"/>
       <c r="B20" s="70"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
       <c r="E20" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F20" s="34" t="s">
         <v>58</v>
@@ -2696,7 +2710,7 @@
     </row>
     <row r="22" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B22" s="62" t="s">
         <v>16</v>
@@ -2708,7 +2722,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F22" s="38" t="s">
         <v>54</v>
@@ -2848,10 +2862,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -2883,8 +2897,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="77"/>
-      <c r="B9" s="79"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="25" t="s">
         <v>9</v>
       </c>
@@ -2914,7 +2928,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="77"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
@@ -2961,7 +2975,7 @@
     </row>
     <row r="12" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="59" t="s">
         <v>16</v>
@@ -2973,7 +2987,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>60</v>
@@ -2996,7 +3010,7 @@
     </row>
     <row r="14" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" s="64" t="s">
         <v>16</v>
@@ -3026,7 +3040,7 @@
         <v>49</v>
       </c>
       <c r="K14" s="39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3138,10 +3152,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -3173,8 +3187,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="77"/>
-      <c r="B9" s="79"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="25" t="s">
         <v>9</v>
       </c>
@@ -3204,7 +3218,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="77"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="15" t="s">
         <v>16</v>
       </c>
@@ -3362,7 +3376,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="72" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="72"/>
       <c r="C6" s="72"/>
@@ -3411,10 +3425,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="78" t="s">
+      <c r="A8" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="79" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="40" t="s">
@@ -3430,7 +3444,7 @@
         <v>54</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H8" s="40" t="s">
         <v>52</v>
@@ -3446,8 +3460,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="77"/>
-      <c r="B9" s="81"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="52" t="s">
         <v>52</v>
       </c>
@@ -3461,7 +3475,7 @@
         <v>53</v>
       </c>
       <c r="G9" s="52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H9" s="52" t="s">
         <v>52</v>
@@ -3477,8 +3491,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="77"/>
-      <c r="B10" s="79"/>
+      <c r="A10" s="78"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="25" t="s">
         <v>9</v>
       </c>
@@ -3508,8 +3522,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="36" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="77"/>
-      <c r="B11" s="80" t="s">
+      <c r="A11" s="78"/>
+      <c r="B11" s="81" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -3525,7 +3539,7 @@
         <v>55</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H11" s="34" t="s">
         <v>52</v>
@@ -3541,8 +3555,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="77"/>
-      <c r="B12" s="80"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="52" t="s">
         <v>52</v>
       </c>
@@ -3556,7 +3570,7 @@
         <v>53</v>
       </c>
       <c r="G12" s="52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H12" s="52" t="s">
         <v>52</v>
@@ -3702,7 +3716,7 @@
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="71" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="70" t="s">
         <v>16</v>
@@ -3711,7 +3725,7 @@
         <v>52</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>23</v>
@@ -3732,7 +3746,7 @@
         <v>49</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -3742,7 +3756,7 @@
         <v>52</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" s="40" t="s">
         <v>23</v>
@@ -3773,7 +3787,7 @@
         <v>52</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>23</v>
@@ -3804,7 +3818,7 @@
         <v>52</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E11" s="53" t="s">
         <v>23</v>
@@ -3843,7 +3857,7 @@
     </row>
     <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="70" t="s">
         <v>16</v>
@@ -3852,7 +3866,7 @@
         <v>52</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" s="39" t="s">
         <v>23</v>
@@ -3873,7 +3887,7 @@
         <v>49</v>
       </c>
       <c r="K13" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -3883,7 +3897,7 @@
         <v>52</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E14" s="40" t="s">
         <v>23</v>
@@ -3914,7 +3928,7 @@
         <v>52</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>23</v>
@@ -3945,7 +3959,7 @@
         <v>52</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E16" s="53" t="s">
         <v>23</v>
@@ -3984,7 +3998,7 @@
     </row>
     <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="70" t="s">
         <v>16</v>
@@ -3993,7 +4007,7 @@
         <v>52</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" s="40" t="s">
         <v>23</v>
@@ -4024,7 +4038,7 @@
         <v>52</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" s="35" t="s">
         <v>23</v>
@@ -4063,7 +4077,7 @@
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="71" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B21" s="70" t="s">
         <v>16</v>
@@ -4072,7 +4086,7 @@
         <v>52</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E21" s="40" t="s">
         <v>23</v>
@@ -4103,7 +4117,7 @@
         <v>52</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E22" s="35" t="s">
         <v>23</v>
@@ -4142,14 +4156,14 @@
     </row>
     <row r="24" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B24" s="70"/>
       <c r="C24" s="40" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E24" s="40" t="s">
         <v>23</v>
@@ -4158,7 +4172,7 @@
         <v>54</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H24" s="40" t="s">
         <v>52</v>
@@ -4180,7 +4194,7 @@
         <v>52</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E25" s="35" t="s">
         <v>23</v>
@@ -4189,7 +4203,7 @@
         <v>55</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H25" s="35" t="s">
         <v>52</v>
@@ -4211,7 +4225,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E26" s="53" t="s">
         <v>23</v>
@@ -4220,7 +4234,7 @@
         <v>53</v>
       </c>
       <c r="G26" s="52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H26" s="52" t="s">
         <v>52</v>
@@ -4250,17 +4264,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="A6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>